<commit_message>
This commit includes the following: - Updates to utility functions - Updates to analyzer - Adding some tests
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval_by_QUESTION.xlsx
+++ b/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval_by_QUESTION.xlsx
@@ -465,10 +465,10 @@
         <v>0.6189327249996216</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.02351246133036713</v>
+        <v>8.43769498715119e-17</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01081937260331701</v>
+        <v>1.576516694967722e-16</v>
       </c>
       <c r="G2" t="n">
         <v>99</v>
@@ -520,10 +520,10 @@
         <v>0.6112970223483144</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.01163706704162387</v>
+        <v>0.01149607432881209</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02677520802357803</v>
+        <v>0.01543341287607883</v>
       </c>
       <c r="G3" t="n">
         <v>97.5</v>
@@ -575,10 +575,10 @@
         <v>0.6447383440763595</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.03011239319855386</v>
+        <v>-0.006754119518834534</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>-0.01028894191738561</v>
       </c>
       <c r="G4" t="n">
         <v>100</v>
@@ -630,10 +630,10 @@
         <v>0.6211045560552616</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.02839618570846824</v>
+        <v>-0.005058824988670463</v>
       </c>
       <c r="F5" t="n">
-        <v>0.05355041604715606</v>
+        <v>0.04115576766954331</v>
       </c>
       <c r="G5" t="n">
         <v>100</v>
@@ -685,10 +685,10 @@
         <v>0.5863017624324911</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.02215272365427458</v>
+        <v>0.001108556945570738</v>
       </c>
       <c r="F6" t="n">
-        <v>0.05355041604715606</v>
+        <v>0.04115576766954331</v>
       </c>
       <c r="G6" t="n">
         <v>100</v>
@@ -740,10 +740,10 @@
         <v>0.62967958704328</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.02407640855637574</v>
+        <v>-0.0007916867668774308</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.08032562407073457</v>
+        <v>-0.08745600629777898</v>
       </c>
       <c r="G7" t="n">
         <v>97.5</v>

</xml_diff>

<commit_message>
This is a big commit that includes the following changes: - Updates to analyzer and comparer to use DSM with subgroups. - Updates to comparison header and evaluation_by_group notebooks. - Additions to utility functions, especially SMD - Updates to docs - Updating all of the tests
</commit_message>
<xml_diff>
--- a/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval_by_QUESTION.xlsx
+++ b/tests/data/experiments/lr-eval-with-xlsx-output/output/lr_eval_with_xlsx_output_eval_by_QUESTION.xlsx
@@ -370,27 +370,27 @@
       <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>DSM.scale_trim</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>DSM.scale_trim_round</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>N</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>R2.scale_trim</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>RMSE.scale_trim</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>SMD.scale_trim</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>SMD.scale_trim_round</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -456,19 +456,19 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>8.43769498715119e-17</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.576516694967722e-16</v>
+      </c>
+      <c r="D2" t="n">
         <v>200</v>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>0.5493203316759327</v>
       </c>
-      <c r="D2" t="n">
+      <c r="F2" t="n">
         <v>0.6189327249996216</v>
-      </c>
-      <c r="E2" t="n">
-        <v>8.43769498715119e-17</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.576516694967722e-16</v>
       </c>
       <c r="G2" t="n">
         <v>99</v>
@@ -511,19 +511,19 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>0.01149607432881209</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.01543341287607883</v>
+      </c>
+      <c r="D3" t="n">
         <v>40</v>
       </c>
-      <c r="C3" t="n">
+      <c r="E3" t="n">
         <v>0.5603717064330405</v>
       </c>
-      <c r="D3" t="n">
+      <c r="F3" t="n">
         <v>0.6112970223483144</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.01149607432881209</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.01543341287607883</v>
       </c>
       <c r="G3" t="n">
         <v>97.5</v>
@@ -566,19 +566,19 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>-0.006754119518834534</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.01028894191738561</v>
+      </c>
+      <c r="D4" t="n">
         <v>40</v>
       </c>
-      <c r="C4" t="n">
+      <c r="E4" t="n">
         <v>0.510955844326675</v>
       </c>
-      <c r="D4" t="n">
+      <c r="F4" t="n">
         <v>0.6447383440763595</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-0.006754119518834534</v>
-      </c>
-      <c r="F4" t="n">
-        <v>-0.01028894191738561</v>
       </c>
       <c r="G4" t="n">
         <v>100</v>
@@ -621,19 +621,19 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>-0.005058824988670463</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.04115576766954331</v>
+      </c>
+      <c r="D5" t="n">
         <v>40</v>
       </c>
-      <c r="C5" t="n">
+      <c r="E5" t="n">
         <v>0.5461519181734076</v>
       </c>
-      <c r="D5" t="n">
+      <c r="F5" t="n">
         <v>0.6211045560552616</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-0.005058824988670463</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.04115576766954331</v>
       </c>
       <c r="G5" t="n">
         <v>100</v>
@@ -676,19 +676,19 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>0.001108556945570738</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.04115576766954331</v>
+      </c>
+      <c r="D6" t="n">
         <v>40</v>
       </c>
-      <c r="C6" t="n">
+      <c r="E6" t="n">
         <v>0.5955885216100645</v>
       </c>
-      <c r="D6" t="n">
+      <c r="F6" t="n">
         <v>0.5863017624324911</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.001108556945570738</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.04115576766954331</v>
       </c>
       <c r="G6" t="n">
         <v>100</v>
@@ -731,19 +731,19 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>-0.0007916867668774308</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.08745600629777898</v>
+      </c>
+      <c r="D7" t="n">
         <v>40</v>
       </c>
-      <c r="C7" t="n">
+      <c r="E7" t="n">
         <v>0.5335336678364757</v>
       </c>
-      <c r="D7" t="n">
+      <c r="F7" t="n">
         <v>0.62967958704328</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-0.0007916867668774308</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-0.08745600629777898</v>
       </c>
       <c r="G7" t="n">
         <v>97.5</v>

</xml_diff>